<commit_message>
Calibrated variables based on component lifetimes
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Repositories\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="SoCDTtiNTY-psgr" sheetId="2" r:id="rId2"/>
     <sheet name="SoCDTtiNTY-frgt" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -462,14 +462,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -477,47 +477,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -534,15 +534,17 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" customWidth="1"/>
+    <col min="2" max="8" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -568,160 +570,202 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>7.5999999999999998E-2</v>
+        <f>1/13</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="C2">
-        <v>7.5999999999999998E-2</v>
+        <f t="shared" ref="C2:H2" si="0">1/13</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="D2">
-        <v>7.5999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="E2">
-        <v>7.5999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="F2">
-        <v>7.5999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="G2">
-        <v>7.5999999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H2">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>4.3499999999999997E-2</v>
+        <f>1/23</f>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="C3">
-        <v>4.3499999999999997E-2</v>
+        <f t="shared" ref="C3:H3" si="1">1/23</f>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="D3">
-        <v>4.3499999999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="E3">
-        <v>4.3499999999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="F3">
-        <v>4.3499999999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="G3">
-        <v>4.3499999999999997E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="H3">
-        <v>4.3499999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>4.1599999999999998E-2</v>
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
-        <v>4.1599999999999998E-2</v>
+        <f t="shared" ref="C4:H4" si="2">1/24</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D4">
-        <v>4.1599999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E4">
-        <v>4.1599999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F4">
-        <v>4.1599999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G4">
-        <v>4.1599999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H4">
-        <v>4.1599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
-        <v>2.9000000000000001E-2</v>
+        <f>1/34</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="C5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" ref="C5:H5" si="3">1/34</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="F5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="G5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="H5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>2.9819999999999999E-2</v>
+        <f>1/33</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="C6">
-        <v>2.9819999999999999E-2</v>
+        <f t="shared" ref="C6:H6" si="4">1/33</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="D6">
-        <v>2.9819999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E6">
-        <v>2.9819999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="F6">
-        <v>2.9819999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="G6">
-        <v>2.9819999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="H6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
-        <v>5.8700000000000002E-2</v>
+        <f>1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="C7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" ref="C7:H7" si="5">1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H7">
-        <v>5.8700000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>
@@ -736,15 +780,17 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" customWidth="1"/>
+    <col min="2" max="8" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -770,137 +816,172 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>7.0000000000000007E-2</v>
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="C2">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" ref="C2:H2" si="0">1/14</f>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="D2">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="E2">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="F2">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="G2">
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="H2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>3.5000000000000003E-2</v>
+        <f>1/28</f>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" ref="C3:H3" si="1">1/28</f>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="D3">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="E3">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="F3">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="G3">
-        <v>3.5000000000000003E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="H3">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>4.2000000000000003E-2</v>
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4">
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" ref="C4:H4" si="2">1/24</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D4">
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E4">
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F4">
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G4">
-        <v>4.2000000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5">
-        <v>2.9000000000000001E-2</v>
+        <f>1/34</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="C5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" ref="C5:H5" si="3">1/34</f>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="F5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="G5">
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="H5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.9411764705882353E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>3.0300000000000001E-2</v>
+        <f>1/33</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="C6">
-        <v>3.0300000000000001E-2</v>
+        <f t="shared" ref="C6:H6" si="4">1/33</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="D6">
-        <v>3.0300000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="E6">
-        <v>3.0300000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="F6">
-        <v>3.0300000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="G6">
-        <v>3.0300000000000001E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="H6">
-        <v>3.0300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>